<commit_message>
send intermediate results to cloud server
</commit_message>
<xml_diff>
--- a/model/model_zoo/model_info.xlsx
+++ b/model/model_zoo/model_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\code2space_controller\model_zoo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227167E7-48C5-4CB7-B063-7B4D3C09147E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683B04E0-1483-4163-A2C3-F687461C8054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="8390" xr2:uid="{FDC729BF-409F-4777-86D3-D256668EC7B4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>conv1</t>
   </si>
@@ -94,11 +94,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>server_latency</t>
+    <t>pi_latency</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>pi_latency</t>
+    <t>server_t4_latency</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>server_gpu_latency</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>server_cpu_latency</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -138,12 +146,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -175,7 +189,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -184,6 +198,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -498,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438032AC-FD14-4F3F-AE18-C9FAA57BC63E}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -511,7 +528,7 @@
     <col min="5" max="5" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -522,13 +539,20 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -547,8 +571,14 @@
       <c r="F2">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1E-4</v>
+      </c>
+      <c r="H2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -567,8 +597,14 @@
       <c r="F3">
         <v>6.1798561151079105E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>1.5999999999999973E-3</v>
+      </c>
+      <c r="H3">
+        <v>4.4866197183098516E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -587,8 +623,14 @@
       <c r="F4">
         <v>6.762589928057559E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>1.6061538461538431E-3</v>
+      </c>
+      <c r="H4">
+        <v>5.1598591549295702E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -607,8 +649,14 @@
       <c r="F5">
         <v>2.084172661870502E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>2.8515384615384635E-3</v>
+      </c>
+      <c r="H5">
+        <v>2.1180281690140825E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -627,8 +675,14 @@
       <c r="F6">
         <v>4.4618705035971203E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>4.0338461538461578E-3</v>
+      </c>
+      <c r="H6">
+        <v>3.9108450704225368E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -647,8 +701,14 @@
       <c r="F7">
         <v>7.5086330935251787E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>5.421538461538462E-3</v>
+      </c>
+      <c r="H7">
+        <v>6.307535211267605E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -667,8 +727,14 @@
       <c r="F8">
         <v>9.3863309352518014E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>7.0653846153846253E-3</v>
+      </c>
+      <c r="H8">
+        <v>7.6457042253521082E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -687,8 +753,14 @@
       <c r="F9">
         <v>9.4597122302158294E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>7.1230769230769316E-3</v>
+      </c>
+      <c r="H9">
+        <v>6.6581690140845085E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -706,6 +778,12 @@
       </c>
       <c r="F10">
         <v>9.6115107913668976E-3</v>
+      </c>
+      <c r="G10">
+        <v>7.1784615384615459E-3</v>
+      </c>
+      <c r="H10">
+        <v>5.7695070422535265E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>